<commit_message>
Add arrays-easy compplete CN code
</commit_message>
<xml_diff>
--- a/striver-a2z-sheet.xlsx
+++ b/striver-a2z-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\striver-a2z-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8410DE5-B169-427C-92AA-8BAF24199748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBB2F6B-C503-4018-87FB-6BB96EC8659A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="28">
   <si>
     <t>S.no</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>CN</t>
+  </si>
+  <si>
+    <t>Move all Zeros to the end of the array</t>
+  </si>
+  <si>
+    <t>Union of Two Sorted Arrays</t>
+  </si>
+  <si>
+    <t>Count Maximum Consecutive One’s in the array</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Find the number that appears once, and the other numbers twice</t>
+  </si>
+  <si>
+    <t>Longest Subarray with given Sum K(Positives)</t>
+  </si>
+  <si>
+    <t>V Imp</t>
+  </si>
+  <si>
+    <t>24-12-2023</t>
+  </si>
+  <si>
+    <t>Longest Subarray with sum K | [Postives and Negatives]</t>
   </si>
 </sst>
 </file>
@@ -120,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +184,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -186,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -196,6 +229,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -480,13 +514,13 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -631,71 +665,133 @@
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -784,8 +880,14 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{61EA6706-98A1-4D03-A35E-97CEEC978AD3}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{9435CBED-8D1C-4554-B996-35956F7E5F80}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{BB49DE46-90E6-4BC4-ADAB-23E817B1BB7B}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{359C4EEF-DB6B-421C-A11D-E5A9A018B9D0}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{4F11D0C3-FA98-4B5D-8074-E87706337F1B}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{263111F9-C9D9-4ACF-8D58-8923D8666303}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{CC26400E-7BF1-464B-876D-8E0897EF486F}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{CE77EE96-F377-422D-8CB7-C28E2BADA536}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{93C6A76E-2C71-45F7-9056-0713FF63374D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add binary search code
</commit_message>
<xml_diff>
--- a/striver-a2z-sheet.xlsx
+++ b/striver-a2z-sheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\striver-a2z-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946E0270-EC0A-4CB7-80E7-C31754A9DC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C06283-F749-44B9-A93D-4F360A64CC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays-Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Arrays-Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Arrays-Hard" sheetId="3" r:id="rId3"/>
+    <sheet name="BinarySearch - 1D Arrays" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
   <si>
     <t>S.no</t>
   </si>
@@ -236,13 +237,40 @@
   </si>
   <si>
     <t>Learn both approaches</t>
+  </si>
+  <si>
+    <t>Find Missing and Repeating numbers</t>
+  </si>
+  <si>
+    <t>Maximum Product Subarray in an Array</t>
+  </si>
+  <si>
+    <t>Count inversions in an array</t>
+  </si>
+  <si>
+    <t>Reverse Pairs</t>
+  </si>
+  <si>
+    <t>Modification of Inversion count</t>
+  </si>
+  <si>
+    <t>Binary Search to find X in sorted Arrays</t>
+  </si>
+  <si>
+    <t>Implement Lower Bound</t>
+  </si>
+  <si>
+    <t>Implement Upper Bound</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +297,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,22 +393,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -388,6 +417,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -672,7 +707,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,28 +719,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -721,10 +756,10 @@
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -743,10 +778,10 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -765,10 +800,10 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -787,10 +822,10 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -809,7 +844,7 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -831,7 +866,7 @@
       <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -853,7 +888,7 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -875,7 +910,7 @@
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -897,7 +932,7 @@
       <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -911,7 +946,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="2"/>
@@ -919,7 +954,7 @@
       <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -943,7 +978,7 @@
       <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="18" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -965,7 +1000,7 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="17" t="s">
         <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1070,43 +1105,43 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:G6"/>
+      <selection activeCell="F8" sqref="F8:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="18"/>
+    <col min="4" max="4" width="9.140625" style="13"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1118,14 +1153,14 @@
         <v>29</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="16"/>
+      <c r="D2" s="11"/>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1143,16 +1178,16 @@
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1170,14 +1205,14 @@
         <v>35</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="16"/>
+      <c r="D4" s="11"/>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1193,14 +1228,14 @@
         <v>36</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="16"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -1216,14 +1251,14 @@
         <v>38</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="16"/>
+      <c r="D6" s="11"/>
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -1239,14 +1274,14 @@
         <v>40</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="16"/>
+      <c r="D7" s="11"/>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -1264,16 +1299,16 @@
       <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -1289,14 +1324,14 @@
         <v>44</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="16"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -1305,27 +1340,27 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="11">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12" t="s">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="11" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="G10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1335,19 +1370,19 @@
         <v>47</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="11" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="11" t="s">
+      <c r="G11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="7" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="2"/>
@@ -1360,43 +1395,43 @@
         <v>48</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="16"/>
+      <c r="D12" s="11"/>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="11" t="s">
+      <c r="G12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>49</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="7">
         <v>12</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="11" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="11"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1406,14 +1441,14 @@
         <v>51</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="16"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -1448,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96699F9A-B078-41D6-BA58-96E1DF1DD8B0}">
-  <dimension ref="A1:I80"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,31 +1497,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1502,10 +1537,10 @@
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -1525,10 +1560,10 @@
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1548,10 +1583,10 @@
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1571,13 +1606,13 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="19">
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="14">
         <v>45292</v>
       </c>
       <c r="I5" s="2"/>
@@ -1594,13 +1629,13 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="19">
+      <c r="G6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="14">
         <v>45292</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1619,13 +1654,13 @@
       <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="19">
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="14">
         <v>45292</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1644,13 +1679,13 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="19">
+      <c r="G8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="14">
         <v>45323</v>
       </c>
       <c r="I8" s="2"/>
@@ -1665,38 +1700,40 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="19">
+        <v>18</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="14">
         <v>45323</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="19">
+      <c r="G10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="14">
         <v>45323</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1707,45 +1744,75 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="14">
+        <v>45352</v>
+      </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="14">
+        <v>45352</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="3" t="s">
+        <v>69</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="14">
+        <v>45413</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -1756,9 +1823,7 @@
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -2472,17 +2537,6 @@
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{CBDBC36B-105C-47AD-80AE-7F30C29C592F}"/>
@@ -2492,10 +2546,248 @@
     <hyperlink ref="B6" r:id="rId5" xr:uid="{AAF92567-A84E-4A7D-A845-29279CC64152}"/>
     <hyperlink ref="B7" r:id="rId6" xr:uid="{CA076557-71E8-4A9C-99B0-E654ACC9FE8B}"/>
     <hyperlink ref="B8" r:id="rId7" xr:uid="{D0EB014C-9F2E-4242-8BAE-D7A2BF854395}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{4F3516A2-6A0E-43B0-83CA-63543BD44725}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{497CA1E5-3A8C-4A42-BEA4-315BA3C7C713}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{497CA1E5-3A8C-4A42-BEA4-315BA3C7C713}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{C8208A4C-7034-4A74-AEBE-04BE10A5B8BB}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{8FE5D25D-984B-423B-85E3-C3728D3BFA19}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{B77A9B7A-48D4-4874-81B8-C6E4F2C08571}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{F9350CAE-6A6D-441A-98BB-E39A25694382}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AF0D50-963F-4938-A68F-979C677948E1}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="14">
+        <v>45444</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="14">
+        <v>45444</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="14">
+        <v>45444</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="14">
+        <v>45444</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{E98D7E32-C0C5-4ACE-80BA-D0E20343F015}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{83BF74BC-CC15-4A82-91F1-320BF72FC7A5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{1E68AAB6-138B-4945-965C-B25631A51528}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{C67439B4-4AA6-4F78-9D06-ED017ED18DFC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BS on 1D array codes
</commit_message>
<xml_diff>
--- a/striver-a2z-sheet.xlsx
+++ b/striver-a2z-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\striver-a2z-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C06283-F749-44B9-A93D-4F360A64CC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FAB1F5-D1C6-430C-A7E6-82A9547485A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="78">
   <si>
     <t>S.no</t>
   </si>
@@ -264,6 +264,15 @@
   </si>
   <si>
     <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Floor and Ceil in Sorted Array</t>
+  </si>
+  <si>
+    <t>First and Last Occurrences in Array</t>
+  </si>
+  <si>
+    <t>Count Occurrences in Sorted Array</t>
   </si>
 </sst>
 </file>
@@ -2562,7 +2571,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,39 +2705,69 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="14">
+        <v>45474</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="3" t="s">
+        <v>76</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="14">
+        <v>45474</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="14">
+        <v>45474</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2787,7 +2826,11 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{83BF74BC-CC15-4A82-91F1-320BF72FC7A5}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{1E68AAB6-138B-4945-965C-B25631A51528}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{C67439B4-4AA6-4F78-9D06-ED017ED18DFC}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{B91DB037-86B5-4E27-871B-004F59A2E93F}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{9004B5A7-A011-4E8C-A2FE-1359ECAC55B0}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{8C987E24-A751-4131-9E8B-3673F828CE12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add BS on answer code
</commit_message>
<xml_diff>
--- a/striver-a2z-sheet.xlsx
+++ b/striver-a2z-sheet.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\striver-a2z-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D16FCD-E51C-4327-8644-98FF872200E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89732B6B-6F16-4697-B2FF-07AB0BB6FDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arrays-Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Arrays-Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Arrays-Hard" sheetId="3" r:id="rId3"/>
     <sheet name="BinarySearch - 1D Arrays" sheetId="4" r:id="rId4"/>
+    <sheet name="Binary Search - Answers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="93">
   <si>
     <t>S.no</t>
   </si>
@@ -289,6 +290,24 @@
   </si>
   <si>
     <t>Find out how many times the array has been rotated</t>
+  </si>
+  <si>
+    <t>Koko  Eating Bananas</t>
+  </si>
+  <si>
+    <t>19/2/2024</t>
+  </si>
+  <si>
+    <t>Finding Sqrt of a number using Binary Search</t>
+  </si>
+  <si>
+    <t>Nth Root of a Number using Binary Search</t>
+  </si>
+  <si>
+    <t>Minimum days to make M bouquets</t>
+  </si>
+  <si>
+    <t>Find the Smallest Divisor Given a Threshold</t>
   </si>
 </sst>
 </file>
@@ -418,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -451,6 +470,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2589,8 +2609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6AF0D50-963F-4938-A68F-979C677948E1}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2957,4 +2977,343 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A89263-B576-4ED2-B3B2-7E23ED72548B}">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{896C5F8D-FB0F-4DAF-A4C3-B325C761F976}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{ADA25173-F706-4508-AE75-0D9DF5AFE0B2}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{57B00E68-32FB-44C3-BE47-8BD8FBC72F20}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{47399862-5E8F-4824-A98F-6F73606A84A0}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{4021A606-0F49-4205-AEB3-09575DD03CA7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add code for BinarySearch on Ans
</commit_message>
<xml_diff>
--- a/striver-a2z-sheet.xlsx
+++ b/striver-a2z-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Code\striver-a2z-workspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89732B6B-6F16-4697-B2FF-07AB0BB6FDC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E827EC7-0AC8-48C8-BECA-9D6856E5E689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="98">
   <si>
     <t>S.no</t>
   </si>
@@ -308,6 +308,21 @@
   </si>
   <si>
     <t>Find the Smallest Divisor Given a Threshold</t>
+  </si>
+  <si>
+    <t>Capacity to Ship Packages within D Days</t>
+  </si>
+  <si>
+    <t>Kth Missing Positive Number</t>
+  </si>
+  <si>
+    <t>21/2/2024</t>
+  </si>
+  <si>
+    <t>make note</t>
+  </si>
+  <si>
+    <t>Aggressive Cows</t>
   </si>
 </sst>
 </file>
@@ -444,7 +459,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -471,6 +485,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -755,7 +770,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +819,7 @@
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -826,7 +841,7 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -848,7 +863,7 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -870,7 +885,7 @@
       <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -892,7 +907,7 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -914,7 +929,7 @@
       <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -936,7 +951,7 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -958,7 +973,7 @@
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -980,7 +995,7 @@
       <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -994,7 +1009,7 @@
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="2"/>
@@ -1002,7 +1017,7 @@
       <c r="E11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1026,7 +1041,7 @@
       <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1048,7 +1063,7 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="16" t="s">
         <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1159,7 +1174,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="54.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="13"/>
+    <col min="4" max="4" width="9.140625" style="12"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
   </cols>
@@ -1174,7 +1189,7 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1201,11 +1216,11 @@
         <v>29</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="11"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1226,13 +1241,13 @@
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -1253,11 +1268,11 @@
         <v>35</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="11"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -1276,11 +1291,11 @@
         <v>36</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="11"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
@@ -1299,11 +1314,11 @@
         <v>38</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="10"/>
       <c r="E6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
@@ -1322,11 +1337,11 @@
         <v>40</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="11"/>
+      <c r="D7" s="10"/>
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
@@ -1347,13 +1362,13 @@
       <c r="C8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -1372,11 +1387,11 @@
         <v>44</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="10"/>
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1388,27 +1403,27 @@
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>9</v>
-      </c>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="16" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="I10" s="7"/>
+      <c r="I10" s="6"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1418,19 +1433,19 @@
         <v>47</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="7" t="s">
+      <c r="G11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>46</v>
       </c>
       <c r="I11" s="2"/>
@@ -1443,43 +1458,43 @@
         <v>48</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="11"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="G12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="19" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="7"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -1489,11 +1504,11 @@
         <v>51</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="11"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
@@ -1554,7 +1569,7 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -1585,7 +1600,7 @@
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
@@ -1608,10 +1623,10 @@
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1631,10 +1646,10 @@
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -1654,13 +1669,13 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="14">
+      <c r="G5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="13">
         <v>45292</v>
       </c>
       <c r="I5" s="2"/>
@@ -1677,13 +1692,13 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="14">
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="13">
         <v>45292</v>
       </c>
       <c r="I6" s="2" t="s">
@@ -1702,13 +1717,13 @@
       <c r="E7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H7" s="13">
         <v>45292</v>
       </c>
       <c r="I7" s="2" t="s">
@@ -1727,13 +1742,13 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="14">
+      <c r="G8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="13">
         <v>45323</v>
       </c>
       <c r="I8" s="2"/>
@@ -1750,13 +1765,13 @@
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="13">
         <v>45323</v>
       </c>
       <c r="I9" s="2" t="s">
@@ -1775,13 +1790,13 @@
       <c r="E10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="14">
+      <c r="H10" s="13">
         <v>45323</v>
       </c>
       <c r="I10" s="2" t="s">
@@ -1800,13 +1815,13 @@
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="13">
         <v>45352</v>
       </c>
       <c r="I11" s="2"/>
@@ -1823,13 +1838,13 @@
       <c r="E12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>45352</v>
       </c>
       <c r="I12" s="2"/>
@@ -1846,13 +1861,13 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="14">
+      <c r="H13" s="13">
         <v>45413</v>
       </c>
       <c r="I13" s="2" t="s">
@@ -2610,13 +2625,13 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14:H15"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="48.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2629,7 +2644,7 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -2641,7 +2656,7 @@
       <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -2660,13 +2675,13 @@
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="20">
         <v>45444</v>
       </c>
       <c r="I2" s="2"/>
@@ -2683,13 +2698,13 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <v>45444</v>
       </c>
       <c r="I3" s="2"/>
@@ -2706,13 +2721,13 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <v>45444</v>
       </c>
       <c r="I4" s="2"/>
@@ -2729,13 +2744,13 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="20">
         <v>45444</v>
       </c>
       <c r="I5" s="2"/>
@@ -2752,13 +2767,13 @@
       <c r="E6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="20">
         <v>45474</v>
       </c>
       <c r="I6" s="2"/>
@@ -2775,13 +2790,13 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="20">
         <v>45474</v>
       </c>
       <c r="I7" s="2"/>
@@ -2798,13 +2813,13 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="20">
         <v>45474</v>
       </c>
       <c r="I8" s="2"/>
@@ -2821,13 +2836,13 @@
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>79</v>
       </c>
       <c r="I9" s="2"/>
@@ -2844,13 +2859,13 @@
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>79</v>
       </c>
       <c r="I10" s="2"/>
@@ -2867,13 +2882,13 @@
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>82</v>
       </c>
       <c r="I11" s="2"/>
@@ -2890,13 +2905,13 @@
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="17" t="s">
         <v>25</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>82</v>
       </c>
       <c r="I12" s="2"/>
@@ -2913,13 +2928,13 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>85</v>
       </c>
       <c r="I13" s="2"/>
@@ -2936,13 +2951,13 @@
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>85</v>
       </c>
       <c r="I14" s="2"/>
@@ -2955,7 +2970,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="11"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="2"/>
     </row>
   </sheetData>
@@ -2984,7 +2999,7 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:H6"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,7 +3021,7 @@
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -3018,7 +3033,7 @@
       <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -3037,13 +3052,13 @@
       <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="20" t="s">
         <v>88</v>
       </c>
       <c r="I2" s="2"/>
@@ -3060,13 +3075,13 @@
       <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>88</v>
       </c>
       <c r="I3" s="2"/>
@@ -3083,13 +3098,13 @@
       <c r="E4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="20" t="s">
         <v>88</v>
       </c>
       <c r="I4" s="2"/>
@@ -3106,13 +3121,13 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="21" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="21" t="s">
+      <c r="H5" s="20" t="s">
         <v>88</v>
       </c>
       <c r="I5" s="2"/>
@@ -3129,49 +3144,89 @@
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>88</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>88</v>
+      </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
@@ -3312,8 +3367,11 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{57B00E68-32FB-44C3-BE47-8BD8FBC72F20}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{47399862-5E8F-4824-A98F-6F73606A84A0}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{4021A606-0F49-4205-AEB3-09575DD03CA7}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{16F09965-898C-4353-96FF-21D22809831A}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{56B782D3-4F77-413F-8DE5-A23DBA7DC0C1}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{1D98D242-B066-4A31-B4BC-79A85A9D8184}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>